<commit_message>
Return variable's name if run returns its definition
</commit_message>
<xml_diff>
--- a/Scoring_Sheet.xlsx
+++ b/Scoring_Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="188">
   <si>
     <t xml:space="preserve">INPUT</t>
   </si>
@@ -801,10 +801,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D123" activeCellId="0" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -859,7 +859,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -873,7 +873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
@@ -906,7 +906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>18</v>
       </c>
@@ -916,8 +916,11 @@
       <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>20</v>
       </c>
@@ -927,8 +930,11 @@
       <c r="C9" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>21</v>
       </c>
@@ -938,8 +944,11 @@
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>22</v>
       </c>
@@ -948,6 +957,9 @@
       </c>
       <c r="C11" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,7 +973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>26</v>
       </c>
@@ -971,8 +983,11 @@
       <c r="C13" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>27</v>
       </c>
@@ -982,8 +997,11 @@
       <c r="C14" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>28</v>
       </c>
@@ -993,8 +1011,11 @@
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>29</v>
       </c>
@@ -1003,6 +1024,9 @@
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>32</v>
       </c>
@@ -1026,8 +1050,11 @@
       <c r="C18" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>33</v>
       </c>
@@ -1036,6 +1063,9 @@
       </c>
       <c r="C19" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,7 +1079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>36</v>
       </c>
@@ -1059,8 +1089,11 @@
       <c r="C21" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
@@ -1070,8 +1103,11 @@
       <c r="C22" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>38</v>
       </c>
@@ -1081,8 +1117,11 @@
       <c r="C23" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>39</v>
       </c>
@@ -1091,6 +1130,9 @@
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>57</v>
       </c>
@@ -1334,7 +1376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>73</v>
       </c>
@@ -1344,8 +1386,11 @@
       <c r="C45" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D45" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>75</v>
       </c>
@@ -1355,8 +1400,11 @@
       <c r="C46" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D46" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>77</v>
       </c>
@@ -1366,8 +1414,11 @@
       <c r="C47" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D47" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>79</v>
       </c>
@@ -1377,8 +1428,11 @@
       <c r="C48" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D48" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>81</v>
       </c>
@@ -1387,6 +1441,9 @@
       </c>
       <c r="C49" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,7 +1490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>87</v>
       </c>
@@ -1443,8 +1500,11 @@
       <c r="C54" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D54" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>88</v>
       </c>
@@ -1453,6 +1513,9 @@
       </c>
       <c r="C55" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1466,7 +1529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>91</v>
       </c>
@@ -1476,8 +1539,11 @@
       <c r="C57" s="2" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D57" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>92</v>
       </c>
@@ -1486,6 +1552,9 @@
       </c>
       <c r="C58" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1499,7 +1568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>95</v>
       </c>
@@ -1509,8 +1578,11 @@
       <c r="C60" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D60" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>96</v>
       </c>
@@ -1519,6 +1591,9 @@
       </c>
       <c r="C61" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,7 +1607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>99</v>
       </c>
@@ -1542,8 +1617,11 @@
       <c r="C63" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>100</v>
       </c>
@@ -1553,8 +1631,11 @@
       <c r="C64" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D64" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>101</v>
       </c>
@@ -1563,6 +1644,9 @@
       </c>
       <c r="C65" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,7 +1660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>104</v>
       </c>
@@ -1586,8 +1670,11 @@
       <c r="C67" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D67" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>105</v>
       </c>
@@ -1597,8 +1684,11 @@
       <c r="C68" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D68" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>106</v>
       </c>
@@ -1608,8 +1698,11 @@
       <c r="C69" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D69" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>107</v>
       </c>
@@ -1620,7 +1713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>109</v>
       </c>
@@ -1630,8 +1723,11 @@
       <c r="C71" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D71" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>110</v>
       </c>
@@ -1641,8 +1737,11 @@
       <c r="C72" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D72" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>111</v>
       </c>
@@ -1652,8 +1751,11 @@
       <c r="C73" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D73" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>112</v>
       </c>
@@ -1664,7 +1766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>114</v>
       </c>
@@ -1674,8 +1776,11 @@
       <c r="C75" s="2" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D75" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>115</v>
       </c>
@@ -1685,8 +1790,11 @@
       <c r="C76" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D76" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>116</v>
       </c>
@@ -1697,7 +1805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>118</v>
       </c>
@@ -1707,8 +1815,11 @@
       <c r="C78" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D78" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>119</v>
       </c>
@@ -1718,8 +1829,11 @@
       <c r="C79" s="2" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D79" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>120</v>
       </c>
@@ -1730,7 +1844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>122</v>
       </c>
@@ -1740,8 +1854,11 @@
       <c r="C81" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D81" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>123</v>
       </c>
@@ -1751,8 +1868,11 @@
       <c r="C82" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D82" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>124</v>
       </c>
@@ -1762,8 +1882,11 @@
       <c r="C83" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D83" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>40</v>
       </c>
@@ -1774,7 +1897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>125</v>
       </c>
@@ -1785,7 +1908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>40</v>
       </c>
@@ -1796,7 +1919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>127</v>
       </c>
@@ -1807,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>129</v>
       </c>
@@ -1817,8 +1940,11 @@
       <c r="C88" s="2" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D88" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>131</v>
       </c>
@@ -1829,7 +1955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>133</v>
       </c>
@@ -1839,8 +1965,11 @@
       <c r="C90" s="2" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D90" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>134</v>
       </c>
@@ -1851,7 +1980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>136</v>
       </c>
@@ -1861,8 +1990,11 @@
       <c r="C92" s="2" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D92" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>137</v>
       </c>
@@ -1873,7 +2005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>139</v>
       </c>
@@ -1884,7 +2016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>141</v>
       </c>
@@ -1894,8 +2026,11 @@
       <c r="C95" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D95" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>143</v>
       </c>
@@ -1905,8 +2040,11 @@
       <c r="C96" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D96" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>145</v>
       </c>
@@ -1916,8 +2054,11 @@
       <c r="C97" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D97" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>147</v>
       </c>
@@ -1927,8 +2068,11 @@
       <c r="C98" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D98" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>149</v>
       </c>
@@ -1939,7 +2083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>151</v>
       </c>
@@ -1949,8 +2093,11 @@
       <c r="C100" s="2" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D100" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>152</v>
       </c>
@@ -1960,8 +2107,11 @@
       <c r="C101" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D101" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>40</v>
       </c>
@@ -1972,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>153</v>
       </c>
@@ -1983,7 +2133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>40</v>
       </c>
@@ -2005,15 +2155,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>157</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D106" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>159</v>
       </c>
@@ -2022,6 +2175,9 @@
       </c>
       <c r="C107" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,7 +2191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>162</v>
       </c>
@@ -2045,8 +2201,11 @@
       <c r="C109" s="2" t="n">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D109" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>163</v>
       </c>
@@ -2055,6 +2214,9 @@
       </c>
       <c r="C110" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,7 +2230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>166</v>
       </c>
@@ -2077,6 +2239,9 @@
       </c>
       <c r="C112" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>169</v>
       </c>
@@ -2099,6 +2264,9 @@
       </c>
       <c r="C114" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,7 +2302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>172</v>
       </c>
@@ -2145,7 +2313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>174</v>
       </c>
@@ -2154,6 +2322,9 @@
       </c>
       <c r="C119" s="2" t="n">
         <v>10</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,7 +2374,7 @@
       </c>
       <c r="D125" s="0" t="n">
         <f aca="false">SUMIF(D2:D123,"x",C2:C123)</f>
-        <v>18</v>
+        <v>142</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,6 +2405,7 @@
         <v>187</v>
       </c>
     </row>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Add more unit tests
</commit_message>
<xml_diff>
--- a/Scoring_Sheet.xlsx
+++ b/Scoring_Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="187">
   <si>
     <t xml:space="preserve">INPUT</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">X if passed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student Output</t>
   </si>
   <si>
     <t xml:space="preserve">; Make sure comments work!</t>
@@ -803,8 +800,8 @@
   </sheetPr>
   <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D123" activeCellId="0" sqref="D123"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -812,6 +809,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="64.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,1582 +825,1589 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="C4" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="D17" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="D20" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D25" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>43</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D27" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="D28" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="D30" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="D31" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="D32" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>54</v>
-      </c>
       <c r="D33" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="D34" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="D35" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D36" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="D37" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D38" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="C39" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="C40" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="C41" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="C42" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>70</v>
-      </c>
       <c r="C43" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="C44" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="0" t="s">
-        <v>74</v>
-      </c>
       <c r="C45" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>76</v>
-      </c>
       <c r="C46" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>78</v>
-      </c>
       <c r="C47" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>80</v>
-      </c>
       <c r="C48" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>82</v>
-      </c>
       <c r="C49" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D50" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>84</v>
-      </c>
       <c r="D51" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D52" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="D53" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="D56" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C57" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C58" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="D59" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="0" t="s">
-        <v>98</v>
-      </c>
       <c r="D62" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C63" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C64" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C65" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B66" s="0" t="s">
-        <v>103</v>
-      </c>
       <c r="D66" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C67" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C68" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C69" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B70" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="D70" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C71" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C72" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C73" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B74" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="D74" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C75" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B77" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B77" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="D77" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C78" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B80" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B80" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="D80" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C81" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C82" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C83" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B84" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B84" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D84" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B85" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B85" s="0" t="s">
-        <v>126</v>
-      </c>
       <c r="D85" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B86" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D86" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B87" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B87" s="0" t="s">
-        <v>128</v>
-      </c>
       <c r="D87" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" s="0" t="s">
         <v>129</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>130</v>
       </c>
       <c r="C88" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B89" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B89" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="D89" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C90" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B91" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B91" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="D91" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C92" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B93" s="0" t="s">
-        <v>138</v>
-      </c>
       <c r="D93" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B94" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B94" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="D94" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B95" s="0" t="s">
-        <v>142</v>
-      </c>
       <c r="C95" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B96" s="0" t="s">
-        <v>144</v>
-      </c>
       <c r="C96" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B97" s="0" t="s">
-        <v>146</v>
-      </c>
       <c r="C97" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B98" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B98" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="C98" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B99" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B99" s="0" t="s">
-        <v>150</v>
-      </c>
       <c r="D99" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C100" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C101" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B102" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B102" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D102" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B103" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B103" s="0" t="s">
-        <v>154</v>
-      </c>
       <c r="D103" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B104" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B104" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D104" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B105" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B105" s="0" t="s">
-        <v>156</v>
-      </c>
       <c r="D105" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B106" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B106" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="D106" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C107" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B108" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B108" s="0" t="s">
-        <v>161</v>
-      </c>
       <c r="D108" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C109" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C110" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B111" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B111" s="0" t="s">
-        <v>165</v>
-      </c>
       <c r="D111" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C112" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B113" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B113" s="0" t="s">
-        <v>168</v>
-      </c>
       <c r="D113" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C114" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B115" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B115" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D115" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B116" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B116" s="0" t="s">
-        <v>171</v>
-      </c>
       <c r="D116" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B117" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B117" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D117" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B118" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="B118" s="0" t="s">
-        <v>173</v>
-      </c>
       <c r="D118" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B119" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="B119" s="0" t="s">
-        <v>175</v>
       </c>
       <c r="C119" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B120" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B120" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D120" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B121" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B121" s="0" t="s">
-        <v>177</v>
+      <c r="D121" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B122" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B122" s="0" t="s">
-        <v>179</v>
+      <c r="D122" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C123" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="D123" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C125" s="4" t="n">
         <v>147</v>
       </c>
       <c r="D125" s="0" t="n">
         <f aca="false">SUMIF(D2:D123,"x",C2:C123)</f>
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Update notes.txt and fix typo on scoring sheet
</commit_message>
<xml_diff>
--- a/Scoring_Sheet.xlsx
+++ b/Scoring_Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="188">
   <si>
     <t xml:space="preserve">INPUT</t>
   </si>
@@ -550,7 +550,7 @@
     <t xml:space="preserve">POPULATE-5-POINTS-FOR-THIS-BEING-ANY-VALUE-5</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt; 5-POINTS-FOR-THIS-BEING-7</t>
+    <t xml:space="preserve">&gt; 5-POINTS-FOR-THIS-BEING-5</t>
   </si>
   <si>
     <t xml:space="preserve">populate 11 50</t>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t xml:space="preserve">run - 18 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 5</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL POSSIBLE POINTS:</t>
@@ -800,8 +803,8 @@
   </sheetPr>
   <dimension ref="A1:E208"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B121" activeCellId="0" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2361,7 +2364,7 @@
         <v>179</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C123" s="2" t="n">
         <v>5</v>
@@ -2372,7 +2375,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C125" s="4" t="n">
         <v>147</v>
@@ -2384,30 +2387,30 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C128" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C129" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C131" s="6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>